<commit_message>
Adeguato script al report del 19/02 e aggiornamento risultati
Nella speranza che ISS la finisca con la follia di cambiare
la struttura dei report settimanalmente

Signed-off-by: enricocid <enrico2588@gmail.com>
</commit_message>
<xml_diff>
--- a/dati/dati_ISS_complessivi.xlsx
+++ b/dati/dati_ISS_complessivi.xlsx
@@ -447,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,529 +508,529 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2">
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="B2">
-        <v>395424</v>
+        <v>555697</v>
       </c>
       <c r="C2">
-        <v>68050</v>
+        <v>102729</v>
       </c>
       <c r="D2">
-        <v>1520148</v>
+        <v>2206303</v>
       </c>
       <c r="E2">
-        <v>200146</v>
+        <v>358530</v>
       </c>
       <c r="F2">
-        <v>9564</v>
+        <v>11487</v>
       </c>
       <c r="G2">
-        <v>479</v>
+        <v>681</v>
       </c>
       <c r="H2">
-        <v>9604</v>
+        <v>13000</v>
       </c>
       <c r="I2">
-        <v>955</v>
+        <v>2066</v>
       </c>
       <c r="J2">
-        <v>1368</v>
+        <v>1557</v>
       </c>
       <c r="K2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="L2">
-        <v>663</v>
+        <v>809</v>
       </c>
       <c r="M2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="N2">
-        <v>1443</v>
+        <v>1774</v>
       </c>
       <c r="O2">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="P2">
-        <v>1606</v>
+        <v>1863</v>
       </c>
       <c r="Q2">
-        <v>132</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2">
-        <v>44566</v>
+        <v>44573</v>
       </c>
       <c r="B3">
-        <v>251412</v>
+        <v>395424</v>
       </c>
       <c r="C3">
-        <v>34617</v>
+        <v>68050</v>
       </c>
       <c r="D3">
-        <v>822338</v>
+        <v>1520148</v>
       </c>
       <c r="E3">
-        <v>79260</v>
+        <v>200146</v>
       </c>
       <c r="F3">
-        <v>8278</v>
+        <v>9564</v>
       </c>
       <c r="G3">
-        <v>410</v>
+        <v>479</v>
       </c>
       <c r="H3">
-        <v>8063</v>
+        <v>9604</v>
       </c>
       <c r="I3">
-        <v>546</v>
+        <v>955</v>
       </c>
       <c r="J3">
-        <v>1202</v>
+        <v>1368</v>
       </c>
       <c r="K3">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="L3">
-        <v>614</v>
+        <v>663</v>
       </c>
       <c r="M3">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N3">
-        <v>1170</v>
+        <v>1443</v>
       </c>
       <c r="O3">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P3">
-        <v>1489</v>
+        <v>1606</v>
       </c>
       <c r="Q3">
-        <v>84</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2">
-        <v>44558</v>
+        <v>44566</v>
       </c>
       <c r="B4">
-        <v>170551</v>
+        <v>251412</v>
       </c>
       <c r="C4">
-        <v>14491</v>
+        <v>34617</v>
       </c>
       <c r="D4">
-        <v>385856</v>
+        <v>822338</v>
       </c>
       <c r="E4">
-        <v>20375</v>
+        <v>79260</v>
       </c>
       <c r="F4">
-        <v>7059</v>
+        <v>8278</v>
       </c>
       <c r="G4">
-        <v>358</v>
+        <v>410</v>
       </c>
       <c r="H4">
-        <v>7229</v>
+        <v>8063</v>
       </c>
       <c r="I4">
-        <v>368</v>
+        <v>546</v>
       </c>
       <c r="J4">
-        <v>1036</v>
+        <v>1202</v>
       </c>
       <c r="K4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4">
-        <v>555</v>
+        <v>614</v>
       </c>
       <c r="M4">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N4">
-        <v>994</v>
+        <v>1170</v>
       </c>
       <c r="O4">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="P4">
-        <v>1262</v>
+        <v>1489</v>
       </c>
       <c r="Q4">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="2">
-        <v>44551</v>
+        <v>44558</v>
       </c>
       <c r="B5">
-        <v>140677</v>
+        <v>170551</v>
       </c>
       <c r="C5">
-        <v>9069</v>
+        <v>14491</v>
       </c>
       <c r="D5">
-        <v>254999</v>
+        <v>385856</v>
       </c>
       <c r="E5">
-        <v>7655</v>
+        <v>20375</v>
       </c>
       <c r="F5">
-        <v>5944</v>
+        <v>7059</v>
       </c>
       <c r="G5">
-        <v>316</v>
+        <v>358</v>
       </c>
       <c r="H5">
-        <v>6384</v>
+        <v>7229</v>
       </c>
       <c r="I5">
-        <v>272</v>
+        <v>368</v>
       </c>
       <c r="J5">
-        <v>887</v>
+        <v>1036</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L5">
-        <v>466</v>
+        <v>555</v>
       </c>
       <c r="M5">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="N5">
-        <v>839</v>
+        <v>994</v>
       </c>
       <c r="O5">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="P5">
-        <v>1105</v>
+        <v>1262</v>
       </c>
       <c r="Q5">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="2">
-        <v>44545</v>
+        <v>44551</v>
       </c>
       <c r="B6">
-        <v>114674</v>
+        <v>140677</v>
       </c>
       <c r="C6">
-        <v>7107</v>
+        <v>9069</v>
       </c>
       <c r="D6">
-        <v>198287</v>
+        <v>254999</v>
       </c>
       <c r="E6">
-        <v>4219</v>
+        <v>7655</v>
       </c>
       <c r="F6">
-        <v>5081</v>
+        <v>5944</v>
       </c>
       <c r="G6">
-        <v>284</v>
+        <v>316</v>
       </c>
       <c r="H6">
-        <v>5451</v>
+        <v>6384</v>
       </c>
       <c r="I6">
-        <v>176</v>
+        <v>272</v>
       </c>
       <c r="J6">
-        <v>747</v>
+        <v>887</v>
       </c>
       <c r="K6">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L6">
-        <v>406</v>
+        <v>466</v>
       </c>
       <c r="M6">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N6">
-        <v>722</v>
+        <v>839</v>
       </c>
       <c r="O6">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="P6">
-        <v>991</v>
+        <v>1105</v>
       </c>
       <c r="Q6">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2">
-        <v>44537</v>
+        <v>44545</v>
       </c>
       <c r="B7">
-        <v>93220</v>
+        <v>114674</v>
       </c>
       <c r="C7">
-        <v>6181</v>
+        <v>7107</v>
       </c>
       <c r="D7">
-        <v>161951</v>
+        <v>198287</v>
       </c>
       <c r="E7">
-        <v>2652</v>
+        <v>4219</v>
       </c>
       <c r="F7">
-        <v>4402</v>
+        <v>5081</v>
       </c>
       <c r="G7">
-        <v>247</v>
+        <v>284</v>
       </c>
       <c r="H7">
-        <v>4653</v>
+        <v>5451</v>
       </c>
       <c r="I7">
-        <v>121</v>
+        <v>176</v>
       </c>
       <c r="J7">
-        <v>618</v>
+        <v>747</v>
       </c>
       <c r="K7">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L7">
-        <v>356</v>
+        <v>406</v>
       </c>
       <c r="M7">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N7">
-        <v>620</v>
+        <v>722</v>
       </c>
       <c r="O7">
+        <v>42</v>
+      </c>
+      <c r="P7">
+        <v>991</v>
+      </c>
+      <c r="Q7">
         <v>29</v>
-      </c>
-      <c r="P7">
-        <v>807</v>
-      </c>
-      <c r="Q7">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="2">
-        <v>44531</v>
+        <v>44537</v>
       </c>
       <c r="B8">
-        <v>75512</v>
+        <v>93220</v>
       </c>
       <c r="C8">
-        <v>5587</v>
+        <v>6181</v>
       </c>
       <c r="D8">
-        <v>128488</v>
+        <v>161951</v>
       </c>
       <c r="E8">
-        <v>1710</v>
+        <v>2652</v>
       </c>
       <c r="F8">
-        <v>3733</v>
+        <v>4402</v>
       </c>
       <c r="G8">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="H8">
-        <v>3845</v>
+        <v>4653</v>
       </c>
       <c r="I8">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="J8">
-        <v>546</v>
+        <v>618</v>
       </c>
       <c r="K8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L8">
-        <v>285</v>
+        <v>356</v>
       </c>
       <c r="M8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N8">
-        <v>515</v>
+        <v>620</v>
       </c>
       <c r="O8">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="P8">
-        <v>690</v>
+        <v>807</v>
       </c>
       <c r="Q8">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2">
-        <v>44524</v>
+        <v>44531</v>
       </c>
       <c r="B9">
-        <v>61908</v>
+        <v>75512</v>
       </c>
       <c r="C9">
-        <v>4260</v>
+        <v>5587</v>
       </c>
       <c r="D9">
-        <v>98228</v>
+        <v>128488</v>
       </c>
       <c r="E9">
-        <v>969</v>
+        <v>1710</v>
       </c>
       <c r="F9">
-        <v>3737</v>
+        <v>3733</v>
       </c>
       <c r="G9">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="H9">
-        <v>3693</v>
+        <v>3845</v>
       </c>
       <c r="I9">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J9">
-        <v>509</v>
+        <v>546</v>
       </c>
       <c r="K9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L9">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="M9">
         <v>3</v>
       </c>
       <c r="N9">
-        <v>449</v>
+        <v>515</v>
       </c>
       <c r="O9">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="P9">
-        <v>555</v>
+        <v>690</v>
       </c>
       <c r="Q9">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="2">
-        <v>44517</v>
+        <v>44524</v>
       </c>
       <c r="B10">
-        <v>50564</v>
+        <v>61908</v>
       </c>
       <c r="C10">
-        <v>3980</v>
+        <v>4260</v>
       </c>
       <c r="D10">
-        <v>72159</v>
+        <v>98228</v>
       </c>
       <c r="E10">
-        <v>537</v>
+        <v>969</v>
       </c>
       <c r="F10">
-        <v>3220</v>
+        <v>3737</v>
       </c>
       <c r="G10">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="H10">
-        <v>2936</v>
+        <v>3693</v>
       </c>
       <c r="I10">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="J10">
-        <v>424</v>
+        <v>509</v>
       </c>
       <c r="K10">
         <v>14</v>
       </c>
       <c r="L10">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>384</v>
+        <v>449</v>
       </c>
       <c r="O10">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="P10">
-        <v>444</v>
+        <v>555</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="2">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B11">
-        <v>40182</v>
+        <v>50564</v>
       </c>
       <c r="C11">
-        <v>3466</v>
+        <v>3980</v>
       </c>
       <c r="D11">
-        <v>52302</v>
+        <v>72159</v>
       </c>
       <c r="E11">
-        <v>286</v>
+        <v>537</v>
       </c>
       <c r="F11">
-        <v>2890</v>
+        <v>3220</v>
       </c>
       <c r="G11">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="H11">
-        <v>2409</v>
+        <v>2936</v>
       </c>
       <c r="I11">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="J11">
-        <v>370</v>
+        <v>424</v>
       </c>
       <c r="K11">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L11">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="O11">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="P11">
-        <v>384</v>
+        <v>444</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1038,52 +1038,52 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="2">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B12">
-        <v>35398</v>
+        <v>40182</v>
       </c>
       <c r="C12">
-        <v>3207</v>
+        <v>3466</v>
       </c>
       <c r="D12">
-        <v>40991</v>
+        <v>52302</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="F12">
-        <v>2696</v>
+        <v>2890</v>
       </c>
       <c r="G12">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H12">
-        <v>2037</v>
+        <v>2409</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J12">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="K12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L12">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>416</v>
+        <v>361</v>
       </c>
       <c r="O12">
         <v>27</v>
       </c>
       <c r="P12">
-        <v>423</v>
+        <v>384</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1091,52 +1091,52 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="2">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B13">
-        <v>34128</v>
+        <v>35398</v>
       </c>
       <c r="C13">
-        <v>3421</v>
+        <v>3207</v>
       </c>
       <c r="D13">
-        <v>34131</v>
+        <v>40991</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>2845</v>
+        <v>2696</v>
       </c>
       <c r="G13">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="H13">
-        <v>1815</v>
+        <v>2037</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="K13">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L13">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>511</v>
+        <v>416</v>
       </c>
       <c r="O13">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="P13">
-        <v>461</v>
+        <v>423</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1144,52 +1144,52 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B14">
-        <v>36194</v>
+        <v>34128</v>
       </c>
       <c r="C14">
-        <v>4127</v>
+        <v>3421</v>
       </c>
       <c r="D14">
-        <v>31514</v>
+        <v>34131</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>3396</v>
+        <v>2845</v>
       </c>
       <c r="G14">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="H14">
-        <v>1954</v>
+        <v>1815</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>414</v>
+        <v>332</v>
       </c>
       <c r="K14">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L14">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>636</v>
+        <v>511</v>
       </c>
       <c r="O14">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P14">
-        <v>511</v>
+        <v>461</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1197,52 +1197,52 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="2">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B15">
-        <v>45790</v>
+        <v>36194</v>
       </c>
       <c r="C15">
-        <v>5352</v>
+        <v>4127</v>
       </c>
       <c r="D15">
-        <v>33496</v>
+        <v>31514</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>4274</v>
+        <v>3396</v>
       </c>
       <c r="G15">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="H15">
-        <v>2133</v>
+        <v>1954</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>515</v>
+        <v>414</v>
       </c>
       <c r="K15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L15">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>775</v>
+        <v>636</v>
       </c>
       <c r="O15">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="P15">
-        <v>578</v>
+        <v>511</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1250,52 +1250,52 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B16">
-        <v>56808</v>
+        <v>45790</v>
       </c>
       <c r="C16">
-        <v>6952</v>
+        <v>5352</v>
       </c>
       <c r="D16">
-        <v>36529</v>
+        <v>33496</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>5224</v>
+        <v>4274</v>
       </c>
       <c r="G16">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="H16">
-        <v>2268</v>
+        <v>2133</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>604</v>
+        <v>515</v>
       </c>
       <c r="K16">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L16">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>888</v>
+        <v>775</v>
       </c>
       <c r="O16">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="P16">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1303,52 +1303,52 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B17">
-        <v>70900</v>
+        <v>56808</v>
       </c>
       <c r="C17">
-        <v>9284</v>
+        <v>6952</v>
       </c>
       <c r="D17">
-        <v>40060</v>
+        <v>36529</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>6160</v>
+        <v>5224</v>
       </c>
       <c r="G17">
-        <v>330</v>
+        <v>278</v>
       </c>
       <c r="H17">
-        <v>2418</v>
+        <v>2268</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>717</v>
+        <v>604</v>
       </c>
       <c r="K17">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L17">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>927</v>
+        <v>888</v>
       </c>
       <c r="O17">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="P17">
-        <v>565</v>
+        <v>580</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1356,52 +1356,52 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B18">
-        <v>86133</v>
+        <v>70900</v>
       </c>
       <c r="C18">
-        <v>11735</v>
+        <v>9284</v>
       </c>
       <c r="D18">
-        <v>44050</v>
+        <v>40060</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>6782</v>
+        <v>6160</v>
       </c>
       <c r="G18">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="H18">
-        <v>2456</v>
+        <v>2418</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>775</v>
+        <v>717</v>
       </c>
       <c r="K18">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L18">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <v>877</v>
+        <v>927</v>
       </c>
       <c r="O18">
         <v>57</v>
       </c>
       <c r="P18">
-        <v>509</v>
+        <v>565</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1409,52 +1409,52 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B19">
-        <v>96900</v>
+        <v>86133</v>
       </c>
       <c r="C19">
-        <v>13728</v>
+        <v>11735</v>
       </c>
       <c r="D19">
-        <v>44990</v>
+        <v>44050</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>6841</v>
+        <v>6782</v>
       </c>
       <c r="G19">
-        <v>404</v>
+        <v>367</v>
       </c>
       <c r="H19">
-        <v>2331</v>
+        <v>2456</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>786</v>
+        <v>775</v>
       </c>
       <c r="K19">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L19">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>770</v>
+        <v>877</v>
       </c>
       <c r="O19">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P19">
-        <v>405</v>
+        <v>509</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -1462,52 +1462,52 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="2">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B20">
-        <v>104890</v>
+        <v>96900</v>
       </c>
       <c r="C20">
-        <v>16129</v>
+        <v>13728</v>
       </c>
       <c r="D20">
-        <v>43775</v>
+        <v>44990</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>6579</v>
+        <v>6841</v>
       </c>
       <c r="G20">
-        <v>450</v>
+        <v>404</v>
       </c>
       <c r="H20">
-        <v>2118</v>
+        <v>2331</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>712</v>
+        <v>786</v>
       </c>
       <c r="K20">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L20">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>571</v>
+        <v>770</v>
       </c>
       <c r="O20">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="P20">
-        <v>280</v>
+        <v>405</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -1515,52 +1515,52 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="2">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B21">
-        <v>107937</v>
+        <v>104890</v>
       </c>
       <c r="C21">
-        <v>18925</v>
+        <v>16129</v>
       </c>
       <c r="D21">
-        <v>40380</v>
+        <v>43775</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>5988</v>
+        <v>6579</v>
       </c>
       <c r="G21">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="H21">
-        <v>1788</v>
+        <v>2118</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>641</v>
+        <v>712</v>
       </c>
       <c r="K21">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L21">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>383</v>
+        <v>571</v>
       </c>
       <c r="O21">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="P21">
-        <v>187</v>
+        <v>280</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -1568,52 +1568,52 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="2">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B22">
-        <v>104405</v>
+        <v>107937</v>
       </c>
       <c r="C22">
-        <v>21703</v>
+        <v>18925</v>
       </c>
       <c r="D22">
-        <v>33894</v>
+        <v>40380</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>5162</v>
+        <v>5988</v>
       </c>
       <c r="G22">
-        <v>509</v>
+        <v>480</v>
       </c>
       <c r="H22">
-        <v>1349</v>
+        <v>1788</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>500</v>
+        <v>641</v>
       </c>
       <c r="K22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L22">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>246</v>
+        <v>383</v>
       </c>
       <c r="O22">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="P22">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -1621,52 +1621,52 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B23">
-        <v>95261</v>
+        <v>104405</v>
       </c>
       <c r="C23">
-        <v>22568</v>
+        <v>21703</v>
       </c>
       <c r="D23">
-        <v>24978</v>
+        <v>33894</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4052</v>
+        <v>5162</v>
       </c>
       <c r="G23">
-        <v>444</v>
+        <v>509</v>
       </c>
       <c r="H23">
-        <v>959</v>
+        <v>1349</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>334</v>
+        <v>500</v>
       </c>
       <c r="K23">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L23">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
-        <v>177</v>
+        <v>246</v>
       </c>
       <c r="O23">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="P23">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -1674,52 +1674,52 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B24">
-        <v>80585</v>
+        <v>95261</v>
       </c>
       <c r="C24">
-        <v>21570</v>
+        <v>22568</v>
       </c>
       <c r="D24">
-        <v>18887</v>
+        <v>24978</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>3067</v>
+        <v>4052</v>
       </c>
       <c r="G24">
-        <v>380</v>
+        <v>444</v>
       </c>
       <c r="H24">
-        <v>627</v>
+        <v>959</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>247</v>
+        <v>334</v>
       </c>
       <c r="K24">
         <v>22</v>
       </c>
       <c r="L24">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="O24">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="P24">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -1727,49 +1727,49 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="2">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B25">
-        <v>60267</v>
+        <v>80585</v>
       </c>
       <c r="C25">
-        <v>17420</v>
+        <v>21570</v>
       </c>
       <c r="D25">
-        <v>12333</v>
+        <v>18887</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>2234</v>
+        <v>3067</v>
       </c>
       <c r="G25">
-        <v>292</v>
+        <v>380</v>
       </c>
       <c r="H25">
-        <v>404</v>
+        <v>627</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>169</v>
+        <v>247</v>
       </c>
       <c r="K25">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="L25">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="O25">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="P25">
         <v>34</v>
@@ -1780,52 +1780,52 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="2">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B26">
-        <v>40729</v>
+        <v>60267</v>
       </c>
       <c r="C26">
-        <v>12032</v>
+        <v>17420</v>
       </c>
       <c r="D26">
-        <v>7277</v>
+        <v>12333</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1619</v>
+        <v>2234</v>
       </c>
       <c r="G26">
-        <v>216</v>
+        <v>292</v>
       </c>
       <c r="H26">
-        <v>280</v>
+        <v>404</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="K26">
         <v>11</v>
       </c>
       <c r="L26">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="O26">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="P26">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -1833,52 +1833,52 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="2">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B27">
-        <v>26284</v>
+        <v>40729</v>
       </c>
       <c r="C27">
-        <v>6813</v>
+        <v>12032</v>
       </c>
       <c r="D27">
-        <v>3805</v>
+        <v>7277</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>1483</v>
+        <v>1619</v>
       </c>
       <c r="G27">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="H27">
-        <v>224</v>
+        <v>280</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="K27">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L27">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>250</v>
+        <v>169</v>
       </c>
       <c r="O27">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P27">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -1886,54 +1886,107 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="2">
+        <v>44398</v>
+      </c>
+      <c r="B28">
+        <v>26284</v>
+      </c>
+      <c r="C28">
+        <v>6813</v>
+      </c>
+      <c r="D28">
+        <v>3805</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1483</v>
+      </c>
+      <c r="G28">
+        <v>199</v>
+      </c>
+      <c r="H28">
+        <v>224</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>117</v>
+      </c>
+      <c r="K28">
+        <v>14</v>
+      </c>
+      <c r="L28">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>250</v>
+      </c>
+      <c r="O28">
+        <v>47</v>
+      </c>
+      <c r="P28">
+        <v>46</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="2">
         <v>44391</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>21089</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>3954</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>2310</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>1880</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>240</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>240</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>147</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>20</v>
       </c>
-      <c r="L28">
+      <c r="L29">
         <v>7</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>357</v>
       </c>
-      <c r="O28">
+      <c r="O29">
         <v>72</v>
       </c>
-      <c r="P28">
+      <c r="P29">
         <v>68</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>0</v>
       </c>
     </row>
@@ -1944,7 +1997,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1993,368 +2046,368 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2">
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="B2">
-        <v>6414467</v>
+        <v>6194434</v>
       </c>
       <c r="C2">
-        <v>1678301</v>
+        <v>1720841</v>
       </c>
       <c r="D2">
-        <v>45917177</v>
+        <v>46094670</v>
       </c>
       <c r="E2">
-        <v>10972555</v>
+        <v>14235354</v>
       </c>
       <c r="F2">
-        <v>6876688</v>
+        <v>6647970</v>
       </c>
       <c r="G2">
-        <v>1504168</v>
+        <v>1566179</v>
       </c>
       <c r="H2">
-        <v>45629089</v>
+        <v>45795796</v>
       </c>
       <c r="I2">
-        <v>5694939</v>
+        <v>8107388</v>
       </c>
       <c r="J2">
-        <v>7031651</v>
+        <v>6862315</v>
       </c>
       <c r="K2">
-        <v>1502381</v>
+        <v>1493790</v>
       </c>
       <c r="L2">
-        <v>45475912</v>
+        <v>45653840</v>
       </c>
       <c r="M2">
-        <v>4133267</v>
+        <v>5699241</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2">
-        <v>44566</v>
+        <v>44573</v>
       </c>
       <c r="B3">
-        <v>6660263</v>
+        <v>6414467</v>
       </c>
       <c r="C3">
-        <v>1578764</v>
+        <v>1678301</v>
       </c>
       <c r="D3">
-        <v>45770918</v>
+        <v>45917177</v>
       </c>
       <c r="E3">
-        <v>8102818</v>
+        <v>10972555</v>
       </c>
       <c r="F3">
+        <v>6876688</v>
+      </c>
+      <c r="G3">
+        <v>1504168</v>
+      </c>
+      <c r="H3">
+        <v>45629089</v>
+      </c>
+      <c r="I3">
+        <v>5694939</v>
+      </c>
+      <c r="J3">
         <v>7031651</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>1502381</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>45475912</v>
       </c>
-      <c r="I3">
+      <c r="M3">
         <v>4133267</v>
-      </c>
-      <c r="J3">
-        <v>7160934</v>
-      </c>
-      <c r="K3">
-        <v>1577260</v>
-      </c>
-      <c r="L3">
-        <v>45271750</v>
-      </c>
-      <c r="M3">
-        <v>3060479</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2">
-        <v>44558</v>
+        <v>44566</v>
       </c>
       <c r="B4">
-        <v>6876688</v>
+        <v>6660263</v>
       </c>
       <c r="C4">
-        <v>1504168</v>
+        <v>1578764</v>
       </c>
       <c r="D4">
-        <v>45629089</v>
+        <v>45770918</v>
       </c>
       <c r="E4">
-        <v>5694939</v>
+        <v>8102818</v>
       </c>
       <c r="F4">
+        <v>7031651</v>
+      </c>
+      <c r="G4">
+        <v>1502381</v>
+      </c>
+      <c r="H4">
+        <v>45475912</v>
+      </c>
+      <c r="I4">
+        <v>4133267</v>
+      </c>
+      <c r="J4">
         <v>7160934</v>
       </c>
-      <c r="G4">
+      <c r="K4">
         <v>1577260</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>45271750</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>3060479</v>
-      </c>
-      <c r="J4">
-        <v>7291722</v>
-      </c>
-      <c r="K4">
-        <v>1749607</v>
-      </c>
-      <c r="L4">
-        <v>44968615</v>
-      </c>
-      <c r="M4">
-        <v>2189265</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2">
-        <v>44551</v>
+        <v>44558</v>
       </c>
       <c r="B5">
-        <v>7031651</v>
+        <v>6876688</v>
       </c>
       <c r="C5">
-        <v>1502381</v>
+        <v>1504168</v>
       </c>
       <c r="D5">
-        <v>45475912</v>
+        <v>45629089</v>
       </c>
       <c r="E5">
-        <v>4133267</v>
+        <v>5694939</v>
       </c>
       <c r="F5">
+        <v>7160934</v>
+      </c>
+      <c r="G5">
+        <v>1577260</v>
+      </c>
+      <c r="H5">
+        <v>45271750</v>
+      </c>
+      <c r="I5">
+        <v>3060479</v>
+      </c>
+      <c r="J5">
         <v>7291722</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <v>1749607</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>44968615</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>2189265</v>
-      </c>
-      <c r="J5">
-        <v>7404599</v>
-      </c>
-      <c r="K5">
-        <v>1981131</v>
-      </c>
-      <c r="L5">
-        <v>44624214</v>
-      </c>
-      <c r="M5">
-        <v>1594076</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2">
-        <v>44545</v>
+        <v>44551</v>
       </c>
       <c r="B6">
-        <v>7160934</v>
+        <v>7031651</v>
       </c>
       <c r="C6">
-        <v>1577260</v>
+        <v>1502381</v>
       </c>
       <c r="D6">
-        <v>45271750</v>
+        <v>45475912</v>
       </c>
       <c r="E6">
-        <v>3060479</v>
+        <v>4133267</v>
       </c>
       <c r="F6">
+        <v>7291722</v>
+      </c>
+      <c r="G6">
+        <v>1749607</v>
+      </c>
+      <c r="H6">
+        <v>44968615</v>
+      </c>
+      <c r="I6">
+        <v>2189265</v>
+      </c>
+      <c r="J6">
         <v>7404599</v>
       </c>
-      <c r="G6">
+      <c r="K6">
         <v>1981131</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>44624214</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>1594076</v>
-      </c>
-      <c r="J6">
-        <v>7586013</v>
-      </c>
-      <c r="K6">
-        <v>2222672</v>
-      </c>
-      <c r="L6">
-        <v>44201259</v>
-      </c>
-      <c r="M6">
-        <v>1016007</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="2">
-        <v>44537</v>
+        <v>44545</v>
       </c>
       <c r="B7">
-        <v>7291722</v>
+        <v>7160934</v>
       </c>
       <c r="C7">
-        <v>1749607</v>
+        <v>1577260</v>
       </c>
       <c r="D7">
-        <v>44968615</v>
+        <v>45271750</v>
       </c>
       <c r="E7">
-        <v>2189265</v>
+        <v>3060479</v>
       </c>
       <c r="F7">
+        <v>7404599</v>
+      </c>
+      <c r="G7">
+        <v>1981131</v>
+      </c>
+      <c r="H7">
+        <v>44624214</v>
+      </c>
+      <c r="I7">
+        <v>1594076</v>
+      </c>
+      <c r="J7">
         <v>7586013</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>2222672</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>44201259</v>
       </c>
-      <c r="I7">
+      <c r="M7">
         <v>1016007</v>
-      </c>
-      <c r="J7">
-        <v>7862567</v>
-      </c>
-      <c r="K7">
-        <v>2422756</v>
-      </c>
-      <c r="L7">
-        <v>43724619</v>
-      </c>
-      <c r="M7">
-        <v>570032</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2">
-        <v>44531</v>
+        <v>44537</v>
       </c>
       <c r="B8">
-        <v>7404599</v>
+        <v>7291722</v>
       </c>
       <c r="C8">
-        <v>1981131</v>
+        <v>1749607</v>
       </c>
       <c r="D8">
-        <v>44624214</v>
+        <v>44968615</v>
       </c>
       <c r="E8">
-        <v>1594076</v>
+        <v>2189265</v>
       </c>
       <c r="F8">
+        <v>7586013</v>
+      </c>
+      <c r="G8">
+        <v>2222672</v>
+      </c>
+      <c r="H8">
+        <v>44201259</v>
+      </c>
+      <c r="I8">
+        <v>1016007</v>
+      </c>
+      <c r="J8">
         <v>7862567</v>
       </c>
-      <c r="G8">
+      <c r="K8">
         <v>2422756</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>43724619</v>
       </c>
-      <c r="I8">
+      <c r="M8">
         <v>570032</v>
-      </c>
-      <c r="J8">
-        <v>8302865</v>
-      </c>
-      <c r="K8">
-        <v>2538614</v>
-      </c>
-      <c r="L8">
-        <v>43168463</v>
-      </c>
-      <c r="M8">
-        <v>294719</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2">
-        <v>44524</v>
+        <v>44531</v>
       </c>
       <c r="B9">
-        <v>7586013</v>
+        <v>7404599</v>
       </c>
       <c r="C9">
-        <v>2222672</v>
+        <v>1981131</v>
       </c>
       <c r="D9">
-        <v>44201259</v>
+        <v>44624214</v>
       </c>
       <c r="E9">
-        <v>1016007</v>
+        <v>1594076</v>
       </c>
       <c r="F9">
+        <v>7862567</v>
+      </c>
+      <c r="G9">
+        <v>2422756</v>
+      </c>
+      <c r="H9">
+        <v>43724619</v>
+      </c>
+      <c r="I9">
+        <v>570032</v>
+      </c>
+      <c r="J9">
         <v>8302865</v>
       </c>
-      <c r="G9">
+      <c r="K9">
         <v>2538614</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>43168463</v>
       </c>
-      <c r="I9">
+      <c r="M9">
         <v>294719</v>
-      </c>
-      <c r="J9">
-        <v>8683749</v>
-      </c>
-      <c r="K9">
-        <v>2653423</v>
-      </c>
-      <c r="L9">
-        <v>42672767</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2">
-        <v>44517</v>
+        <v>44524</v>
       </c>
       <c r="B10">
-        <v>7862567</v>
+        <v>7586013</v>
       </c>
       <c r="C10">
-        <v>2422756</v>
+        <v>2222672</v>
       </c>
       <c r="D10">
-        <v>43724619</v>
+        <v>44201259</v>
       </c>
       <c r="E10">
-        <v>570032</v>
+        <v>1016007</v>
       </c>
       <c r="F10">
+        <v>8302865</v>
+      </c>
+      <c r="G10">
+        <v>2538614</v>
+      </c>
+      <c r="H10">
+        <v>43168463</v>
+      </c>
+      <c r="I10">
+        <v>294719</v>
+      </c>
+      <c r="J10">
         <v>8683749</v>
       </c>
-      <c r="G10">
+      <c r="K10">
         <v>2653423</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>42672767</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>9231487</v>
-      </c>
-      <c r="K10">
-        <v>2863195</v>
-      </c>
-      <c r="L10">
-        <v>41915257</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2362,40 +2415,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B11">
-        <v>8302865</v>
+        <v>7862567</v>
       </c>
       <c r="C11">
-        <v>2538614</v>
+        <v>2422756</v>
       </c>
       <c r="D11">
-        <v>43168463</v>
+        <v>43724619</v>
       </c>
       <c r="E11">
-        <v>294719</v>
+        <v>570032</v>
       </c>
       <c r="F11">
+        <v>8683749</v>
+      </c>
+      <c r="G11">
+        <v>2653423</v>
+      </c>
+      <c r="H11">
+        <v>42672767</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>9231487</v>
       </c>
-      <c r="G11">
+      <c r="K11">
         <v>2863195</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>41915257</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>9829232</v>
-      </c>
-      <c r="K11">
-        <v>3259454</v>
-      </c>
-      <c r="L11">
-        <v>40921215</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2403,40 +2456,40 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="2">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B12">
-        <v>8683749</v>
+        <v>8302865</v>
       </c>
       <c r="C12">
-        <v>2653423</v>
+        <v>2538614</v>
       </c>
       <c r="D12">
-        <v>42672767</v>
+        <v>43168463</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>294719</v>
       </c>
       <c r="F12">
+        <v>9231487</v>
+      </c>
+      <c r="G12">
+        <v>2863195</v>
+      </c>
+      <c r="H12">
+        <v>41915257</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>9829232</v>
       </c>
-      <c r="G12">
+      <c r="K12">
         <v>3259454</v>
       </c>
-      <c r="H12">
+      <c r="L12">
         <v>40921215</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>10307179</v>
-      </c>
-      <c r="K12">
-        <v>3862335</v>
-      </c>
-      <c r="L12">
-        <v>39840387</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -2444,40 +2497,40 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B13">
-        <v>9231487</v>
+        <v>8683749</v>
       </c>
       <c r="C13">
-        <v>2863195</v>
+        <v>2653423</v>
       </c>
       <c r="D13">
-        <v>41915257</v>
+        <v>42672767</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
+        <v>9829232</v>
+      </c>
+      <c r="G13">
+        <v>3259454</v>
+      </c>
+      <c r="H13">
+        <v>40921215</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>10307179</v>
       </c>
-      <c r="G13">
+      <c r="K13">
         <v>3862335</v>
       </c>
-      <c r="H13">
+      <c r="L13">
         <v>39840387</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>10942694</v>
-      </c>
-      <c r="K13">
-        <v>4426185</v>
-      </c>
-      <c r="L13">
-        <v>38641022</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2485,40 +2538,40 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B14">
-        <v>9829232</v>
+        <v>9231487</v>
       </c>
       <c r="C14">
-        <v>3259454</v>
+        <v>2863195</v>
       </c>
       <c r="D14">
-        <v>40921215</v>
+        <v>41915257</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
+        <v>10307179</v>
+      </c>
+      <c r="G14">
+        <v>3862335</v>
+      </c>
+      <c r="H14">
+        <v>39840387</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>10942694</v>
       </c>
-      <c r="G14">
+      <c r="K14">
         <v>4426185</v>
       </c>
-      <c r="H14">
+      <c r="L14">
         <v>38641022</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>11786620</v>
-      </c>
-      <c r="K14">
-        <v>4805486</v>
-      </c>
-      <c r="L14">
-        <v>37417795</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2526,40 +2579,40 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B15">
-        <v>10307179</v>
+        <v>9829232</v>
       </c>
       <c r="C15">
-        <v>3862335</v>
+        <v>3259454</v>
       </c>
       <c r="D15">
-        <v>39840387</v>
+        <v>40921215</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
+        <v>10942694</v>
+      </c>
+      <c r="G15">
+        <v>4426185</v>
+      </c>
+      <c r="H15">
+        <v>38641022</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>11786620</v>
       </c>
-      <c r="G15">
+      <c r="K15">
         <v>4805486</v>
       </c>
-      <c r="H15">
+      <c r="L15">
         <v>37417795</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>12581126</v>
-      </c>
-      <c r="K15">
-        <v>5096568</v>
-      </c>
-      <c r="L15">
-        <v>36332207</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2567,40 +2620,40 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="2">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B16">
-        <v>10942694</v>
+        <v>10307179</v>
       </c>
       <c r="C16">
-        <v>4426185</v>
+        <v>3862335</v>
       </c>
       <c r="D16">
-        <v>38641022</v>
+        <v>39840387</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
+        <v>11786620</v>
+      </c>
+      <c r="G16">
+        <v>4805486</v>
+      </c>
+      <c r="H16">
+        <v>37417795</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>12581126</v>
       </c>
-      <c r="G16">
+      <c r="K16">
         <v>5096568</v>
       </c>
-      <c r="H16">
+      <c r="L16">
         <v>36332207</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>13334156</v>
-      </c>
-      <c r="K16">
-        <v>5075930</v>
-      </c>
-      <c r="L16">
-        <v>35599815</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2608,40 +2661,40 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B17">
-        <v>11786620</v>
+        <v>10942694</v>
       </c>
       <c r="C17">
-        <v>4805486</v>
+        <v>4426185</v>
       </c>
       <c r="D17">
-        <v>37417795</v>
+        <v>38641022</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
+        <v>12581126</v>
+      </c>
+      <c r="G17">
+        <v>5096568</v>
+      </c>
+      <c r="H17">
+        <v>36332207</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>13334156</v>
       </c>
-      <c r="G17">
+      <c r="K17">
         <v>5075930</v>
       </c>
-      <c r="H17">
+      <c r="L17">
         <v>35599815</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>14507530</v>
-      </c>
-      <c r="K17">
-        <v>5210293</v>
-      </c>
-      <c r="L17">
-        <v>34292078</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -2649,40 +2702,40 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="2">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B18">
-        <v>12581126</v>
+        <v>11786620</v>
       </c>
       <c r="C18">
-        <v>5096568</v>
+        <v>4805486</v>
       </c>
       <c r="D18">
-        <v>36332207</v>
+        <v>37417795</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
+        <v>13334156</v>
+      </c>
+      <c r="G18">
+        <v>5075930</v>
+      </c>
+      <c r="H18">
+        <v>35599815</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>14507530</v>
       </c>
-      <c r="G18">
+      <c r="K18">
         <v>5210293</v>
       </c>
-      <c r="H18">
+      <c r="L18">
         <v>34292078</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>15656647</v>
-      </c>
-      <c r="K18">
-        <v>6065610</v>
-      </c>
-      <c r="L18">
-        <v>32287644</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2690,40 +2743,40 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="2">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B19">
-        <v>13334156</v>
+        <v>12581126</v>
       </c>
       <c r="C19">
-        <v>5075930</v>
+        <v>5096568</v>
       </c>
       <c r="D19">
-        <v>35599815</v>
+        <v>36332207</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
+        <v>14507530</v>
+      </c>
+      <c r="G19">
+        <v>5210293</v>
+      </c>
+      <c r="H19">
+        <v>34292078</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>15656647</v>
       </c>
-      <c r="G19">
+      <c r="K19">
         <v>6065610</v>
       </c>
-      <c r="H19">
+      <c r="L19">
         <v>32287644</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>16708830</v>
-      </c>
-      <c r="K19">
-        <v>7672393</v>
-      </c>
-      <c r="L19">
-        <v>29628678</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -2731,40 +2784,40 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B20">
-        <v>14507530</v>
+        <v>13334156</v>
       </c>
       <c r="C20">
-        <v>5210293</v>
+        <v>5075930</v>
       </c>
       <c r="D20">
-        <v>34292078</v>
+        <v>35599815</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
+        <v>15656647</v>
+      </c>
+      <c r="G20">
+        <v>6065610</v>
+      </c>
+      <c r="H20">
+        <v>32287644</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>16708830</v>
       </c>
-      <c r="G20">
+      <c r="K20">
         <v>7672393</v>
       </c>
-      <c r="H20">
+      <c r="L20">
         <v>29628678</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>17568325</v>
-      </c>
-      <c r="K20">
-        <v>9940124</v>
-      </c>
-      <c r="L20">
-        <v>26501452</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2772,40 +2825,40 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B21">
-        <v>15656647</v>
+        <v>14507530</v>
       </c>
       <c r="C21">
-        <v>6065610</v>
+        <v>5210293</v>
       </c>
       <c r="D21">
-        <v>32287644</v>
+        <v>34292078</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
+        <v>16708830</v>
+      </c>
+      <c r="G21">
+        <v>7672393</v>
+      </c>
+      <c r="H21">
+        <v>29628678</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>17568325</v>
       </c>
-      <c r="G21">
+      <c r="K21">
         <v>9940124</v>
       </c>
-      <c r="H21">
+      <c r="L21">
         <v>26501452</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>20322806</v>
-      </c>
-      <c r="K21">
-        <v>11341436</v>
-      </c>
-      <c r="L21">
-        <v>22345659</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -2813,40 +2866,40 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="2">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B22">
-        <v>16708830</v>
+        <v>15656647</v>
       </c>
       <c r="C22">
-        <v>7672393</v>
+        <v>6065610</v>
       </c>
       <c r="D22">
-        <v>29628678</v>
+        <v>32287644</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
+        <v>17568325</v>
+      </c>
+      <c r="G22">
+        <v>9940124</v>
+      </c>
+      <c r="H22">
+        <v>26501452</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>20322806</v>
       </c>
-      <c r="G22">
+      <c r="K22">
         <v>11341436</v>
       </c>
-      <c r="H22">
+      <c r="L22">
         <v>22345659</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>21289761</v>
-      </c>
-      <c r="K22">
-        <v>13149676</v>
-      </c>
-      <c r="L22">
-        <v>19570464</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -2854,40 +2907,40 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="2">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B23">
-        <v>17568325</v>
+        <v>16708830</v>
       </c>
       <c r="C23">
-        <v>9940124</v>
+        <v>7672393</v>
       </c>
       <c r="D23">
-        <v>26501452</v>
+        <v>29628678</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
+        <v>20322806</v>
+      </c>
+      <c r="G23">
+        <v>11341436</v>
+      </c>
+      <c r="H23">
+        <v>22345659</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>21289761</v>
       </c>
-      <c r="G23">
+      <c r="K23">
         <v>13149676</v>
       </c>
-      <c r="H23">
+      <c r="L23">
         <v>19570464</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>22879167</v>
-      </c>
-      <c r="K23">
-        <v>13741130</v>
-      </c>
-      <c r="L23">
-        <v>17389604</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2895,40 +2948,40 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B24">
-        <v>20322806</v>
+        <v>17568325</v>
       </c>
       <c r="C24">
-        <v>11341436</v>
+        <v>9940124</v>
       </c>
       <c r="D24">
-        <v>22345659</v>
+        <v>26501452</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
+        <v>21289761</v>
+      </c>
+      <c r="G24">
+        <v>13149676</v>
+      </c>
+      <c r="H24">
+        <v>19570464</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>22879167</v>
       </c>
-      <c r="G24">
+      <c r="K24">
         <v>13741130</v>
       </c>
-      <c r="H24">
+      <c r="L24">
         <v>17389604</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>24745853</v>
-      </c>
-      <c r="K24">
-        <v>13879852</v>
-      </c>
-      <c r="L24">
-        <v>15384196</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2936,40 +2989,40 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B25">
-        <v>21289761</v>
+        <v>20322806</v>
       </c>
       <c r="C25">
-        <v>13149676</v>
+        <v>11341436</v>
       </c>
       <c r="D25">
-        <v>19570464</v>
+        <v>22345659</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
+        <v>22879167</v>
+      </c>
+      <c r="G25">
+        <v>13741130</v>
+      </c>
+      <c r="H25">
+        <v>17389604</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>24745853</v>
       </c>
-      <c r="G25">
+      <c r="K25">
         <v>13879852</v>
       </c>
-      <c r="H25">
+      <c r="L25">
         <v>15384196</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>27065063</v>
-      </c>
-      <c r="K25">
-        <v>13015437</v>
-      </c>
-      <c r="L25">
-        <v>13929401</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2977,40 +3030,40 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="2">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B26">
-        <v>22879167</v>
+        <v>21289761</v>
       </c>
       <c r="C26">
-        <v>13741130</v>
+        <v>13149676</v>
       </c>
       <c r="D26">
-        <v>17389604</v>
+        <v>19570464</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
+        <v>24745853</v>
+      </c>
+      <c r="G26">
+        <v>13879852</v>
+      </c>
+      <c r="H26">
+        <v>15384196</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>27065063</v>
       </c>
-      <c r="G26">
+      <c r="K26">
         <v>13015437</v>
       </c>
-      <c r="H26">
+      <c r="L26">
         <v>13929401</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -3018,28 +3071,28 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="2">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B27">
-        <v>24745853</v>
+        <v>22879167</v>
       </c>
       <c r="C27">
-        <v>13879852</v>
+        <v>13741130</v>
       </c>
       <c r="D27">
-        <v>15384196</v>
+        <v>17389604</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>27065063</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>13015437</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>13929401</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -3059,42 +3112,83 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2">
+        <v>44398</v>
+      </c>
+      <c r="B28">
+        <v>24745853</v>
+      </c>
+      <c r="C28">
+        <v>13879852</v>
+      </c>
+      <c r="D28">
+        <v>15384196</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2">
         <v>44391</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>27065063</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>13015437</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>13929401</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>0</v>
       </c>
     </row>

</xml_diff>